<commit_message>
Changed to single board design
</commit_message>
<xml_diff>
--- a/DOCS/Ranges.xlsx
+++ b/DOCS/Ranges.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B57668-2ABD-4594-9964-8E05613B09D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67542F77-220B-47DD-A7C9-D9539C3CC234}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranges" sheetId="1" r:id="rId1"/>
-    <sheet name="SPI timings" sheetId="2" r:id="rId2"/>
+    <sheet name="Power" sheetId="3" r:id="rId2"/>
+    <sheet name="SPI timings" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="69">
   <si>
     <t>A</t>
   </si>
@@ -636,6 +637,54 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Load FET driver 1</t>
+  </si>
+  <si>
+    <t>Load FET driver 2</t>
+  </si>
+  <si>
+    <t>Bypass On</t>
+  </si>
+  <si>
+    <t>Bypass Off</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>mW</t>
+  </si>
+  <si>
+    <t>Current ADC 1</t>
+  </si>
+  <si>
+    <t>Current ADC 2</t>
+  </si>
+  <si>
+    <t>Voltage ADC</t>
+  </si>
+  <si>
+    <t>Temp ADC</t>
+  </si>
+  <si>
+    <t>Iso</t>
+  </si>
+  <si>
+    <t>MAX743</t>
+  </si>
+  <si>
+    <t>To 5V</t>
+  </si>
+  <si>
+    <t>To 12V</t>
+  </si>
+  <si>
+    <t>Fan</t>
   </si>
 </sst>
 </file>
@@ -645,7 +694,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##0.00E+0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,6 +764,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -742,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -798,10 +856,19 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1084,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1103,20 +1170,20 @@
     <col min="19" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
       <c r="R1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1124,18 +1191,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+    <row r="2" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="R2" s="6">
         <f>49.4/S2+1</f>
         <v>50.4</v>
@@ -1144,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1184,7 +1251,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
@@ -1218,8 +1285,15 @@
       <c r="S4" s="1">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="W4" s="22">
+        <f>2^16*U5/V4</f>
+        <v>50688.384096024005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1276,8 +1350,12 @@
       <c r="S5" s="1">
         <v>1.07</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="3">
+        <f>B5*B7</f>
+        <v>2.3976744186046512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1407,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1379,7 +1457,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
@@ -1436,7 +1514,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1494,7 +1572,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G10" s="9" t="s">
         <v>33</v>
       </c>
@@ -1534,7 +1612,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="3"/>
       <c r="M11" s="5"/>
       <c r="R11" s="6">
@@ -1545,20 +1623,20 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
       <c r="M12" s="5"/>
       <c r="R12" s="6">
         <f t="shared" si="0"/>
@@ -1568,18 +1646,18 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+    <row r="13" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
       <c r="M13" s="5"/>
       <c r="R13" s="6">
         <f t="shared" si="0"/>
@@ -1589,7 +1667,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1623,7 +1701,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>31</v>
       </c>
@@ -1663,7 +1741,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1990,19 +2068,19 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
       <c r="M23" s="5"/>
       <c r="R23" s="6">
         <f t="shared" si="0"/>
@@ -2013,17 +2091,17 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
       <c r="M24" s="5"/>
       <c r="R24" s="6">
         <f t="shared" si="0"/>
@@ -2575,6 +2653,418 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD2F9DA-F989-4F05-B358-67BD5736B8A3}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19">
+        <v>3</v>
+      </c>
+      <c r="C1" s="19">
+        <v>5</v>
+      </c>
+      <c r="D1" s="19">
+        <v>12</v>
+      </c>
+      <c r="E1" s="19">
+        <v>15</v>
+      </c>
+      <c r="F1" s="19">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="6">
+        <f>8.57*3</f>
+        <v>25.71</v>
+      </c>
+      <c r="C10" s="6">
+        <f>14.3*11+21*4</f>
+        <v>241.3</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="6">
+        <f>SUM(B2:B13)</f>
+        <v>29.71</v>
+      </c>
+      <c r="C14" s="6">
+        <f>SUM(C2:C13)</f>
+        <v>271.3</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" ref="D14:F14" si="0">SUM(D2:D13)</f>
+        <v>30.25</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="6">
+        <f>ABS(B14*B1)</f>
+        <v>89.13</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" ref="C15:F15" si="1">ABS(C14*C1)</f>
+        <v>1356.5</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>363</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="6">
+        <f>B14</f>
+        <v>29.71</v>
+      </c>
+      <c r="C16" s="6">
+        <f>SUM(B16,E16,F16,C14)</f>
+        <v>385.01</v>
+      </c>
+      <c r="E16" s="19">
+        <f>E15/0.75/5</f>
+        <v>64</v>
+      </c>
+      <c r="F16" s="19">
+        <f>F15/0.6/5</f>
+        <v>20</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="19">
+        <f>$C$1*B16</f>
+        <v>148.55000000000001</v>
+      </c>
+      <c r="C17" s="6">
+        <f>SUM(B17,C15,E17,F17)</f>
+        <v>1925.05</v>
+      </c>
+      <c r="E17" s="19">
+        <f t="shared" ref="C17:F17" si="2">$C$1*E16</f>
+        <v>320</v>
+      </c>
+      <c r="F17" s="19">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="6">
+        <f>C16</f>
+        <v>385.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="C19" s="19">
+        <f>C18*D1</f>
+        <v>4620.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBB7D5-8A6F-4FB6-B62C-6FEA60EB499C}">
   <dimension ref="A1:E8"/>
   <sheetViews>

</xml_diff>